<commit_message>
Some more paradox links
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/Paradox-KeyLinks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/Paradox-KeyLinks.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="6885" windowWidth="12765" windowHeight="5985"/>
+    <workbookView xWindow="90" yWindow="6945" windowWidth="12765" windowHeight="5925"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Paradox ID</t>
   </si>
@@ -164,6 +164,24 @@
   </si>
   <si>
     <t>Store Outside Temp</t>
+  </si>
+  <si>
+    <t>~RackA\SGr1\RefLevel Measure</t>
+  </si>
+  <si>
+    <t>Refrigerant Level `%rackname`</t>
+  </si>
+  <si>
+    <t>Comp VFD Value `%rackname`</t>
+  </si>
+  <si>
+    <t>Rack B VFD % Measure</t>
+  </si>
+  <si>
+    <t>~A01 POS Freezer #1\Defrost Temp</t>
+  </si>
+  <si>
+    <t>System Defrost Temp `%rackname` `%sgname` `%sysname`</t>
   </si>
 </sst>
 </file>
@@ -539,11 +557,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,123 +581,123 @@
       <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
+      <c r="A2" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
+      <c r="A3" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
+      <c r="A4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
+      <c r="A5" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>2</v>
+      <c r="A6" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>10</v>
+      <c r="A14" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>19</v>
+      <c r="A15" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C16"/>
     </row>
@@ -692,59 +710,59 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>3</v>
+      <c r="A22" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>46</v>
+      <c r="A23" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>45</v>
+      <c r="A24" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -755,9 +773,33 @@
         <v>36</v>
       </c>
     </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:B25">
-    <sortCondition ref="A3"/>
+  <sortState ref="A2:B28">
+    <sortCondition ref="B2:B28"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Major fix on modbus creating
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/Paradox-KeyLinks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/Paradox-KeyLinks.xlsx
@@ -535,14 +535,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>